<commit_message>
gradient boosting added to test
</commit_message>
<xml_diff>
--- a/ML_PL_new/test_scores.xlsx
+++ b/ML_PL_new/test_scores.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,42 +458,57 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>FTR_GB</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>BTTS_gNB</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>BTTS_RF</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>BTTS_DT</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>BTTS_KNN</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>BTTS_GB</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>O/U2.5_gNB</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>O/U2.5_RF</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>O/U2.5_DT</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>O/U2.5_KNN</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>O/U2.5_GB</t>
         </is>
       </c>
     </row>
@@ -504,40 +519,49 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.4984810126582279</v>
+        <v>0.4974050632911393</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5067721518987341</v>
+        <v>0.5082278481012659</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4637341772151898</v>
+        <v>0.4633544303797468</v>
       </c>
       <c r="E2" t="n">
-        <v>0.4713924050632912</v>
+        <v>0.4681012658227848</v>
       </c>
       <c r="F2" t="n">
-        <v>0.590379746835443</v>
+        <v>0.4963291139240507</v>
       </c>
       <c r="G2" t="n">
         <v>0.5965822784810126</v>
       </c>
       <c r="H2" t="n">
-        <v>0.5993037974683544</v>
+        <v>0.600379746835443</v>
       </c>
       <c r="I2" t="n">
-        <v>0.5683544303797469</v>
+        <v>0.6011392405063291</v>
       </c>
       <c r="J2" t="n">
-        <v>0.6203164556962024</v>
+        <v>0.5767088607594937</v>
       </c>
       <c r="K2" t="n">
-        <v>0.6337341772151899</v>
+        <v>0.6322784810126582</v>
       </c>
       <c r="L2" t="n">
-        <v>0.6299367088607595</v>
+        <v>0.6251898734177215</v>
       </c>
       <c r="M2" t="n">
-        <v>0.6150632911392404</v>
+        <v>0.6374683544303796</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.6336075949367088</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.6203164556962025</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0.6518987341772151</v>
       </c>
     </row>
     <row r="3">
@@ -547,40 +571,49 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.05460472991210835</v>
+        <v>0.05006998151802123</v>
       </c>
       <c r="C3" t="n">
-        <v>0.05084519933262131</v>
+        <v>0.05485762118443563</v>
       </c>
       <c r="D3" t="n">
-        <v>0.05619786534563814</v>
+        <v>0.05758093749176584</v>
       </c>
       <c r="E3" t="n">
-        <v>0.05117450939946652</v>
+        <v>0.05181123657631183</v>
       </c>
       <c r="F3" t="n">
-        <v>0.04252643535532329</v>
+        <v>0.05266866728244041</v>
       </c>
       <c r="G3" t="n">
-        <v>0.04222755918949405</v>
+        <v>0.04583020293839912</v>
       </c>
       <c r="H3" t="n">
-        <v>0.05759072506761253</v>
+        <v>0.04422439657662171</v>
       </c>
       <c r="I3" t="n">
-        <v>0.05045768292115342</v>
+        <v>0.05800020770818953</v>
       </c>
       <c r="J3" t="n">
-        <v>0.04752393751875721</v>
+        <v>0.04587111986991489</v>
       </c>
       <c r="K3" t="n">
-        <v>0.04731304235662194</v>
+        <v>0.04530789429936875</v>
       </c>
       <c r="L3" t="n">
-        <v>0.05440407913063352</v>
+        <v>0.04631047581207948</v>
       </c>
       <c r="M3" t="n">
-        <v>0.04952658786098899</v>
+        <v>0.04295970162544888</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.04999595380899909</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.04609625614387271</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.04499134818491073</v>
       </c>
     </row>
     <row r="4">
@@ -590,40 +623,49 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.3544303797468354</v>
+        <v>0.3670886075949367</v>
       </c>
       <c r="C4" t="n">
-        <v>0.3417721518987342</v>
+        <v>0.3670886075949367</v>
       </c>
       <c r="D4" t="n">
-        <v>0.3037974683544304</v>
+        <v>0.2911392405063291</v>
       </c>
       <c r="E4" t="n">
         <v>0.3291139240506329</v>
       </c>
       <c r="F4" t="n">
+        <v>0.3291139240506329</v>
+      </c>
+      <c r="G4" t="n">
         <v>0.4683544303797468</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>0.4810126582278481</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
+        <v>0.4177215189873418</v>
+      </c>
+      <c r="J4" t="n">
         <v>0.4556962025316456</v>
       </c>
-      <c r="I4" t="n">
+      <c r="K4" t="n">
+        <v>0.5063291139240507</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.5063291139240507</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.5189873417721519</v>
+      </c>
+      <c r="N4" t="n">
         <v>0.4556962025316456</v>
       </c>
-      <c r="J4" t="n">
-        <v>0.4810126582278481</v>
-      </c>
-      <c r="K4" t="n">
+      <c r="O4" t="n">
+        <v>0.4683544303797468</v>
+      </c>
+      <c r="P4" t="n">
         <v>0.5189873417721519</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0.4303797468354431</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0.4683544303797468</v>
       </c>
     </row>
     <row r="5">
@@ -639,34 +681,43 @@
         <v>0.4683544303797468</v>
       </c>
       <c r="D5" t="n">
+        <v>0.4177215189873418</v>
+      </c>
+      <c r="E5" t="n">
         <v>0.4303797468354431</v>
       </c>
-      <c r="E5" t="n">
-        <v>0.439873417721519</v>
-      </c>
       <c r="F5" t="n">
-        <v>0.5569620253164557</v>
+        <v>0.4556962025316456</v>
       </c>
       <c r="G5" t="n">
         <v>0.569620253164557</v>
       </c>
       <c r="H5" t="n">
-        <v>0.5664556962025317</v>
+        <v>0.569620253164557</v>
       </c>
       <c r="I5" t="n">
-        <v>0.5316455696202531</v>
+        <v>0.569620253164557</v>
       </c>
       <c r="J5" t="n">
-        <v>0.5822784810126582</v>
+        <v>0.5443037974683544</v>
       </c>
       <c r="K5" t="n">
-        <v>0.6075949367088608</v>
+        <v>0.5949367088607594</v>
       </c>
       <c r="L5" t="n">
         <v>0.5949367088607594</v>
       </c>
       <c r="M5" t="n">
-        <v>0.5822784810126582</v>
+        <v>0.6075949367088608</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.6075949367088608</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.5949367088607594</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.620253164556962</v>
       </c>
     </row>
     <row r="6">
@@ -676,7 +727,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.5063291139240507</v>
+        <v>0.4936708860759494</v>
       </c>
       <c r="C6" t="n">
         <v>0.5063291139240507</v>
@@ -688,28 +739,37 @@
         <v>0.4683544303797468</v>
       </c>
       <c r="F6" t="n">
-        <v>0.5949367088607594</v>
+        <v>0.4936708860759494</v>
       </c>
       <c r="G6" t="n">
-        <v>0.5949367088607594</v>
+        <v>0.6075949367088608</v>
       </c>
       <c r="H6" t="n">
         <v>0.5949367088607594</v>
       </c>
       <c r="I6" t="n">
-        <v>0.569620253164557</v>
+        <v>0.6075949367088608</v>
       </c>
       <c r="J6" t="n">
-        <v>0.620253164556962</v>
+        <v>0.5822784810126582</v>
       </c>
       <c r="K6" t="n">
         <v>0.6329113924050633</v>
       </c>
       <c r="L6" t="n">
+        <v>0.620253164556962</v>
+      </c>
+      <c r="M6" t="n">
         <v>0.6329113924050633</v>
       </c>
-      <c r="M6" t="n">
+      <c r="N6" t="n">
+        <v>0.6329113924050633</v>
+      </c>
+      <c r="O6" t="n">
         <v>0.620253164556962</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.6455696202531646</v>
       </c>
     </row>
     <row r="7">
@@ -719,7 +779,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.5443037974683544</v>
+        <v>0.5316455696202531</v>
       </c>
       <c r="C7" t="n">
         <v>0.5443037974683544</v>
@@ -731,28 +791,37 @@
         <v>0.5063291139240507</v>
       </c>
       <c r="F7" t="n">
-        <v>0.620253164556962</v>
+        <v>0.5316455696202531</v>
       </c>
       <c r="G7" t="n">
         <v>0.6329113924050633</v>
       </c>
       <c r="H7" t="n">
+        <v>0.6329113924050633</v>
+      </c>
+      <c r="I7" t="n">
         <v>0.6455696202531646</v>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>0.6075949367088608</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.6487341772151899</v>
       </c>
       <c r="K7" t="n">
         <v>0.6708860759493671</v>
       </c>
       <c r="L7" t="n">
+        <v>0.6582278481012658</v>
+      </c>
+      <c r="M7" t="n">
         <v>0.6708860759493671</v>
       </c>
-      <c r="M7" t="n">
+      <c r="N7" t="n">
+        <v>0.6708860759493671</v>
+      </c>
+      <c r="O7" t="n">
         <v>0.6455696202531646</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.6835443037974683</v>
       </c>
     </row>
     <row r="8">
@@ -762,40 +831,49 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.6582278481012658</v>
+        <v>0.620253164556962</v>
       </c>
       <c r="C8" t="n">
-        <v>0.6582278481012658</v>
+        <v>0.6708860759493671</v>
       </c>
       <c r="D8" t="n">
-        <v>0.6075949367088608</v>
+        <v>0.6329113924050633</v>
       </c>
       <c r="E8" t="n">
+        <v>0.6329113924050633</v>
+      </c>
+      <c r="F8" t="n">
         <v>0.620253164556962</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>0.6962025316455697</v>
       </c>
-      <c r="G8" t="n">
-        <v>0.6835443037974683</v>
-      </c>
       <c r="H8" t="n">
+        <v>0.7088607594936709</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.7088607594936709</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.7215189873417721</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.759493670886076</v>
+      </c>
+      <c r="L8" t="n">
         <v>0.7468354430379747</v>
       </c>
-      <c r="I8" t="n">
+      <c r="M8" t="n">
         <v>0.759493670886076</v>
       </c>
-      <c r="J8" t="n">
-        <v>0.7848101265822784</v>
-      </c>
-      <c r="K8" t="n">
+      <c r="N8" t="n">
         <v>0.7721518987341772</v>
       </c>
-      <c r="L8" t="n">
+      <c r="O8" t="n">
+        <v>0.7468354430379747</v>
+      </c>
+      <c r="P8" t="n">
         <v>0.759493670886076</v>
-      </c>
-      <c r="M8" t="n">
-        <v>0.7468354430379747</v>
       </c>
     </row>
   </sheetData>
@@ -809,7 +887,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -840,42 +918,57 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>FTR_GB</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>BTTS_gNB</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>BTTS_RF</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>BTTS_DT</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>BTTS_KNN</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>BTTS_GB</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>O/U2.5_gNB</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>O/U2.5_RF</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>O/U2.5_DT</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>O/U2.5_KNN</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>O/U2.5_GB</t>
         </is>
       </c>
     </row>
@@ -886,40 +979,49 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>49.5</v>
+        <v>49.2</v>
       </c>
       <c r="C2" t="n">
-        <v>52</v>
+        <v>52.5</v>
       </c>
       <c r="D2" t="n">
-        <v>39.1</v>
+        <v>39</v>
       </c>
       <c r="E2" t="n">
-        <v>41.4</v>
+        <v>40.4</v>
       </c>
       <c r="F2" t="n">
-        <v>18.1</v>
+        <v>48.9</v>
       </c>
       <c r="G2" t="n">
         <v>19.3</v>
       </c>
       <c r="H2" t="n">
-        <v>19.9</v>
+        <v>20.1</v>
       </c>
       <c r="I2" t="n">
-        <v>13.7</v>
+        <v>20.2</v>
       </c>
       <c r="J2" t="n">
+        <v>15.3</v>
+      </c>
+      <c r="K2" t="n">
+        <v>26.5</v>
+      </c>
+      <c r="L2" t="n">
+        <v>25</v>
+      </c>
+      <c r="M2" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="N2" t="n">
+        <v>26.7</v>
+      </c>
+      <c r="O2" t="n">
         <v>24.1</v>
       </c>
-      <c r="K2" t="n">
-        <v>26.7</v>
-      </c>
-      <c r="L2" t="n">
-        <v>26</v>
-      </c>
-      <c r="M2" t="n">
-        <v>23</v>
+      <c r="P2" t="n">
+        <v>30.4</v>
       </c>
     </row>
     <row r="3">
@@ -929,40 +1031,49 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-83.59999999999999</v>
+        <v>-85</v>
       </c>
       <c r="C3" t="n">
-        <v>-84.7</v>
+        <v>-83.5</v>
       </c>
       <c r="D3" t="n">
-        <v>-83.09999999999999</v>
+        <v>-82.7</v>
       </c>
       <c r="E3" t="n">
-        <v>-84.59999999999999</v>
+        <v>-84.5</v>
       </c>
       <c r="F3" t="n">
-        <v>-91.5</v>
+        <v>-84.2</v>
       </c>
       <c r="G3" t="n">
-        <v>-91.59999999999999</v>
+        <v>-90.8</v>
       </c>
       <c r="H3" t="n">
-        <v>-88.5</v>
+        <v>-91.2</v>
       </c>
       <c r="I3" t="n">
-        <v>-89.90000000000001</v>
+        <v>-88.40000000000001</v>
       </c>
       <c r="J3" t="n">
-        <v>-90.5</v>
+        <v>-90.8</v>
       </c>
       <c r="K3" t="n">
-        <v>-90.5</v>
+        <v>-90.90000000000001</v>
       </c>
       <c r="L3" t="n">
-        <v>-89.09999999999999</v>
+        <v>-90.7</v>
       </c>
       <c r="M3" t="n">
-        <v>-90.09999999999999</v>
+        <v>-91.40000000000001</v>
+      </c>
+      <c r="N3" t="n">
+        <v>-90</v>
+      </c>
+      <c r="O3" t="n">
+        <v>-90.8</v>
+      </c>
+      <c r="P3" t="n">
+        <v>-91</v>
       </c>
     </row>
     <row r="4">
@@ -972,40 +1083,49 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6.3</v>
+        <v>10.1</v>
       </c>
       <c r="C4" t="n">
-        <v>2.5</v>
+        <v>10.1</v>
       </c>
       <c r="D4" t="n">
-        <v>-8.9</v>
+        <v>-12.7</v>
       </c>
       <c r="E4" t="n">
         <v>-1.3</v>
       </c>
       <c r="F4" t="n">
+        <v>-1.3</v>
+      </c>
+      <c r="G4" t="n">
         <v>-6.3</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>-3.8</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
+        <v>-16.5</v>
+      </c>
+      <c r="J4" t="n">
         <v>-8.9</v>
       </c>
-      <c r="I4" t="n">
+      <c r="K4" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="L4" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="M4" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="N4" t="n">
         <v>-8.9</v>
       </c>
-      <c r="J4" t="n">
-        <v>-3.8</v>
-      </c>
-      <c r="K4" t="n">
+      <c r="O4" t="n">
+        <v>-6.3</v>
+      </c>
+      <c r="P4" t="n">
         <v>3.8</v>
-      </c>
-      <c r="L4" t="n">
-        <v>-13.9</v>
-      </c>
-      <c r="M4" t="n">
-        <v>-6.3</v>
       </c>
     </row>
     <row r="5">
@@ -1021,34 +1141,43 @@
         <v>40.5</v>
       </c>
       <c r="D5" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="E5" t="n">
         <v>29.1</v>
       </c>
-      <c r="E5" t="n">
-        <v>32</v>
-      </c>
       <c r="F5" t="n">
-        <v>11.4</v>
+        <v>36.7</v>
       </c>
       <c r="G5" t="n">
         <v>13.9</v>
       </c>
       <c r="H5" t="n">
-        <v>13.3</v>
+        <v>13.9</v>
       </c>
       <c r="I5" t="n">
-        <v>6.3</v>
+        <v>13.9</v>
       </c>
       <c r="J5" t="n">
-        <v>16.5</v>
+        <v>8.9</v>
       </c>
       <c r="K5" t="n">
-        <v>21.5</v>
+        <v>19</v>
       </c>
       <c r="L5" t="n">
         <v>19</v>
       </c>
       <c r="M5" t="n">
-        <v>16.5</v>
+        <v>21.5</v>
+      </c>
+      <c r="N5" t="n">
+        <v>21.5</v>
+      </c>
+      <c r="O5" t="n">
+        <v>19</v>
+      </c>
+      <c r="P5" t="n">
+        <v>24.1</v>
       </c>
     </row>
     <row r="6">
@@ -1058,7 +1187,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>51.9</v>
+        <v>48.1</v>
       </c>
       <c r="C6" t="n">
         <v>51.9</v>
@@ -1070,28 +1199,37 @@
         <v>40.5</v>
       </c>
       <c r="F6" t="n">
-        <v>19</v>
+        <v>48.1</v>
       </c>
       <c r="G6" t="n">
-        <v>19</v>
+        <v>21.5</v>
       </c>
       <c r="H6" t="n">
         <v>19</v>
       </c>
       <c r="I6" t="n">
-        <v>13.9</v>
+        <v>21.5</v>
       </c>
       <c r="J6" t="n">
-        <v>24.1</v>
+        <v>16.5</v>
       </c>
       <c r="K6" t="n">
         <v>26.6</v>
       </c>
       <c r="L6" t="n">
+        <v>24.1</v>
+      </c>
+      <c r="M6" t="n">
         <v>26.6</v>
       </c>
-      <c r="M6" t="n">
+      <c r="N6" t="n">
+        <v>26.6</v>
+      </c>
+      <c r="O6" t="n">
         <v>24.1</v>
+      </c>
+      <c r="P6" t="n">
+        <v>29.1</v>
       </c>
     </row>
     <row r="7">
@@ -1101,7 +1239,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>63.3</v>
+        <v>59.5</v>
       </c>
       <c r="C7" t="n">
         <v>63.3</v>
@@ -1113,28 +1251,37 @@
         <v>51.9</v>
       </c>
       <c r="F7" t="n">
-        <v>24.1</v>
+        <v>59.5</v>
       </c>
       <c r="G7" t="n">
         <v>26.6</v>
       </c>
       <c r="H7" t="n">
+        <v>26.6</v>
+      </c>
+      <c r="I7" t="n">
         <v>29.1</v>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>21.5</v>
-      </c>
-      <c r="J7" t="n">
-        <v>29.7</v>
       </c>
       <c r="K7" t="n">
         <v>34.2</v>
       </c>
       <c r="L7" t="n">
+        <v>31.6</v>
+      </c>
+      <c r="M7" t="n">
         <v>34.2</v>
       </c>
-      <c r="M7" t="n">
+      <c r="N7" t="n">
+        <v>34.2</v>
+      </c>
+      <c r="O7" t="n">
         <v>29.1</v>
+      </c>
+      <c r="P7" t="n">
+        <v>36.7</v>
       </c>
     </row>
     <row r="8">
@@ -1144,40 +1291,49 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>97.5</v>
+        <v>86.09999999999999</v>
       </c>
       <c r="C8" t="n">
-        <v>97.5</v>
+        <v>101.3</v>
       </c>
       <c r="D8" t="n">
-        <v>82.3</v>
+        <v>89.90000000000001</v>
       </c>
       <c r="E8" t="n">
+        <v>89.90000000000001</v>
+      </c>
+      <c r="F8" t="n">
         <v>86.09999999999999</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>39.2</v>
       </c>
-      <c r="G8" t="n">
-        <v>36.7</v>
-      </c>
       <c r="H8" t="n">
+        <v>41.8</v>
+      </c>
+      <c r="I8" t="n">
+        <v>41.8</v>
+      </c>
+      <c r="J8" t="n">
+        <v>44.3</v>
+      </c>
+      <c r="K8" t="n">
+        <v>51.9</v>
+      </c>
+      <c r="L8" t="n">
         <v>49.4</v>
       </c>
-      <c r="I8" t="n">
+      <c r="M8" t="n">
         <v>51.9</v>
       </c>
-      <c r="J8" t="n">
-        <v>57</v>
-      </c>
-      <c r="K8" t="n">
+      <c r="N8" t="n">
         <v>54.4</v>
       </c>
-      <c r="L8" t="n">
+      <c r="O8" t="n">
+        <v>49.4</v>
+      </c>
+      <c r="P8" t="n">
         <v>51.9</v>
-      </c>
-      <c r="M8" t="n">
-        <v>49.4</v>
       </c>
     </row>
   </sheetData>
@@ -1191,7 +1347,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1222,22 +1378,32 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>FTR_GB</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>O/U2.5_gNB</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>O/U2.5_RF</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>O/U2.5_DT</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>O/U2.5_KNN</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>O/U2.5_GB</t>
         </is>
       </c>
     </row>
@@ -1271,6 +1437,12 @@
       <c r="I2" t="n">
         <v>300</v>
       </c>
+      <c r="J2" t="n">
+        <v>300</v>
+      </c>
+      <c r="K2" t="n">
+        <v>300</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -1279,28 +1451,34 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-10.6618476387613</v>
+        <v>-8.33549258465899</v>
       </c>
       <c r="C3" t="n">
-        <v>-23.33182006444249</v>
+        <v>-19.67085744922444</v>
       </c>
       <c r="D3" t="n">
-        <v>-21.28707703331268</v>
+        <v>-17.19022348328681</v>
       </c>
       <c r="E3" t="n">
-        <v>-24.53043954988152</v>
+        <v>-21.98583159884765</v>
       </c>
       <c r="F3" t="n">
-        <v>3.919214693838182</v>
+        <v>-25.47855093993547</v>
       </c>
       <c r="G3" t="n">
-        <v>0.7103331203331084</v>
+        <v>4.475051963100621</v>
       </c>
       <c r="H3" t="n">
-        <v>3.752086544024021</v>
+        <v>1.183489052441255</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.01147609724723367</v>
+        <v>4.440264506146576</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1.037060247171797</v>
+      </c>
+      <c r="K3" t="n">
+        <v>5.182611128559667</v>
       </c>
     </row>
     <row r="4">
@@ -1310,28 +1488,34 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>13.30721767055794</v>
+        <v>10.65040341048969</v>
       </c>
       <c r="C4" t="n">
-        <v>15.23453254560455</v>
+        <v>13.49452794585846</v>
       </c>
       <c r="D4" t="n">
-        <v>14.30676295402742</v>
+        <v>13.05067505494932</v>
       </c>
       <c r="E4" t="n">
-        <v>13.6088432358219</v>
+        <v>12.13864442288408</v>
       </c>
       <c r="F4" t="n">
-        <v>10.5828045036646</v>
+        <v>14.65410307287836</v>
       </c>
       <c r="G4" t="n">
-        <v>10.14905283507087</v>
+        <v>10.34964384037962</v>
       </c>
       <c r="H4" t="n">
-        <v>11.19404629211075</v>
+        <v>9.684320781986543</v>
       </c>
       <c r="I4" t="n">
-        <v>9.955740925617398</v>
+        <v>10.41363468730878</v>
+      </c>
+      <c r="J4" t="n">
+        <v>8.958648321727878</v>
+      </c>
+      <c r="K4" t="n">
+        <v>10.31973280993218</v>
       </c>
     </row>
     <row r="5">
@@ -1341,28 +1525,34 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-50.69160166549455</v>
+        <v>-38.22271468001645</v>
       </c>
       <c r="C5" t="n">
-        <v>-70.56000836834328</v>
+        <v>-62.576647032816</v>
       </c>
       <c r="D5" t="n">
-        <v>-58.19306399439034</v>
+        <v>-60.94657844214715</v>
       </c>
       <c r="E5" t="n">
-        <v>-64.59086117627189</v>
+        <v>-56.37842191290093</v>
       </c>
       <c r="F5" t="n">
-        <v>-24.2244913581558</v>
+        <v>-72.41503743072639</v>
       </c>
       <c r="G5" t="n">
-        <v>-26.38853794603393</v>
+        <v>-27.66962832675908</v>
       </c>
       <c r="H5" t="n">
-        <v>-25.75640625177282</v>
+        <v>-28.23598459712059</v>
       </c>
       <c r="I5" t="n">
-        <v>-31.0785979288037</v>
+        <v>-29.20245926209875</v>
+      </c>
+      <c r="J5" t="n">
+        <v>-26.45552385504812</v>
+      </c>
+      <c r="K5" t="n">
+        <v>-27.66962832675908</v>
       </c>
     </row>
     <row r="6">
@@ -1372,28 +1562,34 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-18.95845743637723</v>
+        <v>-15.17254330629996</v>
       </c>
       <c r="C6" t="n">
-        <v>-33.76579145225514</v>
+        <v>-28.02162266470328</v>
       </c>
       <c r="D6" t="n">
-        <v>-30.24117167921396</v>
+        <v>-26.4406484976103</v>
       </c>
       <c r="E6" t="n">
-        <v>-32.25654497312158</v>
+        <v>-31.14011213103829</v>
       </c>
       <c r="F6" t="n">
-        <v>-2.852940074716061</v>
+        <v>-35.41716570695253</v>
       </c>
       <c r="G6" t="n">
-        <v>-5.190224065304085</v>
+        <v>-2.161147282523468</v>
       </c>
       <c r="H6" t="n">
-        <v>-3.214170095528636</v>
+        <v>-5.471963685094597</v>
       </c>
       <c r="I6" t="n">
-        <v>-6.182961149422108</v>
+        <v>-2.123155510459363</v>
+      </c>
+      <c r="J6" t="n">
+        <v>-4.504321018487849</v>
+      </c>
+      <c r="K6" t="n">
+        <v>-1.410253170161539</v>
       </c>
     </row>
     <row r="7">
@@ -1403,28 +1599,34 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-10.71212985779372</v>
+        <v>-7.955298980566197</v>
       </c>
       <c r="C7" t="n">
-        <v>-23.61515719867285</v>
+        <v>-18.94198887514706</v>
       </c>
       <c r="D7" t="n">
-        <v>-19.89383984374416</v>
+        <v>-16.48022981490216</v>
       </c>
       <c r="E7" t="n">
-        <v>-23.77203708468792</v>
+        <v>-21.27224949026942</v>
       </c>
       <c r="F7" t="n">
-        <v>4.06177396688648</v>
+        <v>-24.67420369192573</v>
       </c>
       <c r="G7" t="n">
-        <v>0.506468194862539</v>
+        <v>4.558164148300445</v>
       </c>
       <c r="H7" t="n">
-        <v>4.887008284650804</v>
+        <v>1.268508260673014</v>
       </c>
       <c r="I7" t="n">
-        <v>0.09297366778424421</v>
+        <v>4.126965459878039</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1.359808983881096</v>
+      </c>
+      <c r="K7" t="n">
+        <v>5.175290314862615</v>
       </c>
     </row>
     <row r="8">
@@ -1434,28 +1636,34 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.9239789058386934</v>
+        <v>-0.4244789575371394</v>
       </c>
       <c r="C8" t="n">
-        <v>-11.13081764404508</v>
+        <v>-10.50899140920108</v>
       </c>
       <c r="D8" t="n">
-        <v>-11.90549231331559</v>
+        <v>-7.838569618802591</v>
       </c>
       <c r="E8" t="n">
-        <v>-15.10840779110202</v>
+        <v>-13.10107099211462</v>
       </c>
       <c r="F8" t="n">
-        <v>10.5222429364861</v>
+        <v>-15.18324506394002</v>
       </c>
       <c r="G8" t="n">
-        <v>6.201288128907822</v>
+        <v>11.54392964133005</v>
       </c>
       <c r="H8" t="n">
-        <v>10.25011967014195</v>
+        <v>7.622170647822144</v>
       </c>
       <c r="I8" t="n">
-        <v>6.777687432125978</v>
+        <v>11.60531976375231</v>
+      </c>
+      <c r="J8" t="n">
+        <v>7.186151140689343</v>
+      </c>
+      <c r="K8" t="n">
+        <v>11.85703828579945</v>
       </c>
     </row>
     <row r="9">
@@ -1465,28 +1673,34 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>19.63006643740352</v>
+        <v>18.24998841398354</v>
       </c>
       <c r="C9" t="n">
-        <v>16.08521593677523</v>
+        <v>15.55098470067806</v>
       </c>
       <c r="D9" t="n">
-        <v>12.32571283986941</v>
+        <v>15.1445810611478</v>
       </c>
       <c r="E9" t="n">
-        <v>9.222844631897578</v>
+        <v>8.717009939740446</v>
       </c>
       <c r="F9" t="n">
-        <v>33.11553737590789</v>
+        <v>11.45456757226248</v>
       </c>
       <c r="G9" t="n">
-        <v>29.51566496156354</v>
+        <v>32.35565549616786</v>
       </c>
       <c r="H9" t="n">
-        <v>32.6952380126245</v>
+        <v>31.7102343601391</v>
       </c>
       <c r="I9" t="n">
-        <v>25.65326492465637</v>
+        <v>32.39580169034406</v>
+      </c>
+      <c r="J9" t="n">
+        <v>24.02101019025249</v>
+      </c>
+      <c r="K9" t="n">
+        <v>41.20693309117006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ML_PL: added weather variables
</commit_message>
<xml_diff>
--- a/ML_PL_new/test_scores.xlsx
+++ b/ML_PL_new/test_scores.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000"/>
   </bookViews>
   <sheets>
     <sheet name="describe" sheetId="1" r:id="rId1"/>
@@ -170,6 +170,444 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="hu-HU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>describe_relative!$B$1:$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>FTR_gNB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FTR_RF</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FTR_DT</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>FTR_KNN</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FTR_GB</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>BTTS_gNB</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>BTTS_RF</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>BTTS_DT</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>BTTS_KNN</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>BTTS_GB</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>O/U2.5_gNB</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>O/U2.5_RF</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>O/U2.5_DT</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>O/U2.5_KNN</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>O/U2.5_GB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>describe_relative!$B$2:$P$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>49.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>52.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>48.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>26.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>27.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>26.7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>24.1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>30.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-90CF-4FB6-97B9-392F91974B6B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>describe_relative!$B$1:$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>FTR_gNB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FTR_RF</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FTR_DT</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>FTR_KNN</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FTR_GB</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>BTTS_gNB</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>BTTS_RF</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>BTTS_DT</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>BTTS_KNN</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>BTTS_GB</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>O/U2.5_gNB</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>O/U2.5_RF</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>O/U2.5_DT</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>O/U2.5_KNN</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>O/U2.5_GB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>describe_relative!$B$6:$P$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>48.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>48.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>26.6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24.1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>26.6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>26.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>24.1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>29.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-90CF-4FB6-97B9-392F91974B6B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="409147816"/>
+        <c:axId val="409147488"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="409147816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="hu-HU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="409147488"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="409147488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="hu-HU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="409147816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="hu-HU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="hu-HU"/>
@@ -516,6 +954,46 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="16">
   <a:schemeClr val="accent3"/>
 </cs:colorStyle>
@@ -1024,7 +1502,545 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>290512</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>595312</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagram 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1346,7 +2362,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
@@ -1759,7 +2775,7 @@
   <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2163,6 +3179,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2170,7 +3187,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
@@ -2767,7 +3784,7 @@
         <v>0.23101251156941191</v>
       </c>
       <c r="C18">
-        <f t="shared" ref="B18:K18" si="6">C9/79</f>
+        <f t="shared" ref="C18:K18" si="6">C9/79</f>
         <v>0.19684790760351975</v>
       </c>
       <c r="D18">

</xml_diff>